<commit_message>
revision y correccion de los archivos: cronograma preliminar y lista de posibles riesgos
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt de seguimiento de fechas1.xlsx
+++ b/Diagrama de Gantt de seguimiento de fechas1.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9834073-FD0D-41E2-A222-F2DDDB72C98F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28710" windowHeight="12495" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28710" windowHeight="12495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos del gráfico" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <definedName name="IntervaloDeFechas">{15,30,45,60,75,90,105,120}</definedName>
     <definedName name="Seguimiento_hoy">'Datos del gráfico'!$E$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -318,7 +319,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
@@ -886,7 +887,7 @@
     <cellStyle name="Cálculo" xfId="18" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="20" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="19" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="6"/>
+    <cellStyle name="Date" xfId="6" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="12" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="24" builtinId="29" customBuiltin="1"/>
@@ -1206,7 +1207,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Date Tracking Gantt Chart" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Date Tracking Gantt Chart" pivot="0" count="5">
+    <tableStyle name="Date Tracking Gantt Chart" pivot="0" count="5" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="27"/>
       <tableStyleElement type="headerRow" dxfId="26"/>
       <tableStyleElement type="firstColumn" dxfId="25"/>
@@ -1249,38 +1250,77 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:noFill/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60C11BC5-C658-4BA1-9D0E-AF276F6E03B7}" type="CELLRANGE">
+                    <a:fld id="{0BB05C34-38AA-4976-8BD3-B227078524B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1293,7 +1333,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1304,18 +1343,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44732A01-C013-4A7D-BEA2-5B0670E3EC16}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F5A73E63-8E13-45C0-BD2B-8BFC821468EC}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1328,7 +1366,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1340,18 +1377,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F166A7D-4019-4B10-88C3-0E807BF12991}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{87FE84C6-257C-4C60-BF83-09384290AC00}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1364,7 +1400,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1376,18 +1411,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DE6090C-FFBD-4C95-AF50-FA5EAC13D642}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{DBABED4C-D9DC-4404-8327-032488DD08EC}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1400,7 +1434,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1412,18 +1445,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5E0B120-2E18-4D49-AA3A-0E5651052B69}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{E91A42AB-4557-49EF-A0B2-FC5D548AA79B}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1436,7 +1468,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1448,18 +1479,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8EB03C1-1D15-427B-9E51-18F37727A941}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2612D2E9-2606-486D-86F2-9D576719D04B}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1472,7 +1502,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1484,18 +1513,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10C7FC7E-F5A9-4FAF-B83C-2B8DFC531576}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9591B0B5-6FE9-4AFB-9BC3-4277521C0336}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1508,7 +1536,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1532,11 +1559,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="accent2">
-                        <a:lumMod val="60000"/>
-                        <a:lumOff val="40000"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1544,7 +1570,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-CO"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1557,7 +1583,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1581,19 +1606,19 @@
                     <c:v>3</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>3</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>3</c:v>
                   </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0</c:v>
-                  </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1609,11 +1634,10 @@
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="101600" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
@@ -1628,25 +1652,25 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>43710</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43724</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43724</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43731</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>43738</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>43738</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43745</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43745</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43785</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43785</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43785</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,13 +1694,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1689,16 +1713,25 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
+                    <c:v>Inicio de Diseño Relacional y Diagrama de Procesos</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Modelo Relacional y Diagrama De Procesos.</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Identificacion de Sedes y Tablas a Fragmentar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Lista de Sedes y Fragmentaciones Correspondientes</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Diagrama de Despliegue y Componentes</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Especificacion de Lenguajes a Usar</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="6">
                     <c:v>Casos de Uso</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>inicio de Contruccion de la Plataforma</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Inicio Construccion de Base de Datos En el lenguaje planteado</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1724,81 +1757,76 @@
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:noFill/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                    <a:spAutoFit/>
-                  </a:bodyPr>
+                  <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="bg2"/>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:fld id="{5F5C573C-459C-46A3-9C4C-17B0E0A18EF1}" type="CELLRANGE">
+                    <a:fld id="{28CF966E-A047-419F-9147-0F69B18D1A78}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
-                      <a:pPr>
-                        <a:defRPr sz="1100">
-                          <a:solidFill>
-                            <a:schemeClr val="bg2"/>
-                          </a:solidFill>
-                        </a:defRPr>
-                      </a:pPr>
+                      <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="bg2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -1808,7 +1836,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1819,7 +1846,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1837,9 +1863,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000015-CCF3-4D6B-A363-E3E4CAC6EE6E}"/>
                 </c:ext>
@@ -1861,9 +1885,8 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1871,7 +1894,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-CO"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1897,12 +1920,13 @@
             <c:val val="100"/>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="bg2"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:miter lim="800000"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1914,10 +1938,10 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>43738</c:v>
+                  <c:v>43710</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43738</c:v>
+                  <c:v>43710</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1960,36 +1984,73 @@
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln w="9525" cap="rnd">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58195A35-745F-4F5E-8700-294EBD65562A}" type="CELLRANGE">
+                    <a:fld id="{E1CC9545-71FA-4566-87B0-A6389675E876}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2002,7 +2063,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -2013,18 +2073,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0B709E7-679D-4F0A-B4EE-277D54AE767B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7BA379D0-AD88-4DB9-AB67-F08695CF2783}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2037,8 +2096,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2048,18 +2107,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03094994-2EF7-4406-9FE4-58BCA6719A4A}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{206F6B56-87CA-449E-84D4-66B1FF8B7257}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2072,8 +2130,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2083,18 +2141,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7FDE183-4E2A-4BB0-AC74-ED9883F59FDB}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{25A85D7A-90A7-45ED-B1CA-520BAD36F755}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2107,8 +2164,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2118,18 +2175,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8E4EAAF-DF56-4F96-9991-6A9C45EAEAEA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F3FCC510-817C-4AEA-8457-74475CEED3A6}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2142,8 +2198,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2153,18 +2209,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D02565A8-1AE2-4A3A-852C-87B619EBC292}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9AD22681-0692-4F94-9A5B-74F78CA3C9BC}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2177,8 +2232,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2188,18 +2243,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3279CC20-95F2-4986-86FD-64B2227ABC31}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D5C61B16-910B-463E-AD87-CAA2B1142CE4}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2212,8 +2266,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2223,18 +2277,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73DE774C-42E0-4DDD-964C-7FBCD971B685}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{3FE08E4D-B743-4059-8BC8-472A1AF0E091}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2247,8 +2300,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2258,18 +2311,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C3F0AA1-DFBD-4D3C-B1F7-3D6BAABB7F01}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{6E09BF64-9130-45FB-B247-93969996B09A}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2282,8 +2334,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2293,18 +2345,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2F98D90-B84C-44CA-A470-4E940FC56DD4}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D3EF1124-0167-47A4-86AE-05BF0B0BF06F}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2317,8 +2368,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2328,18 +2379,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1950157A-4483-4F72-B23A-C6C96D911852}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{81ADDA0A-47CA-4434-906B-6A823ECE7539}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2352,8 +2402,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2363,18 +2413,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B79871D-31DC-4F32-9917-3A85688CDC25}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{826F3AD6-B256-4472-B34B-1587E80B7C90}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2387,8 +2436,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2398,18 +2447,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83EEE301-C6E3-49A4-B64D-EDAD886B92B1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{3415C571-C357-46CE-855E-C67CCFAB3502}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2422,8 +2470,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2433,18 +2481,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="13"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBCF1AB2-8991-445C-A094-12C0AFCEB5DE}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D15BD65A-878B-44CA-A883-07934BFDF83D}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2457,8 +2504,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2468,18 +2515,17 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="14"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA52AC63-6384-46F1-BC88-AD73E7FFD584}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{18F98D9B-3997-4D15-8DC2-1B42BCADB20E}" type="CELLRANGE">
+                      <a:rPr lang="es-CO"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="es-CO"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2492,8 +2538,8 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2540,16 +2586,18 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="accent6"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-CO"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2574,49 +2622,49 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>43768</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43789</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2628,10 +2676,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2682,12 +2730,6 @@
                 <c15:f>'Datos de gráf. dinám. (ocultos)'!$G$18:$G$33</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="16"/>
-                  <c:pt idx="0">
-                    <c:v>Presentacion Beta Plataforma (50 - 60 % del proyecto)</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Fase 2 Programa Completo (80 - 90 % completado)</c:v>
-                  </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -2719,7 +2761,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2732,11 +2777,12 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="101600" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2745,16 +2791,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="594340336"/>
@@ -2767,12 +2815,56 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="594342512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -2787,7 +2879,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2795,14 +2886,31 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="tx1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
       <a:noFill/>
-      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -2813,7 +2921,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2865,62 +2973,66 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -2929,9 +3041,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2950,14 +3061,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2966,20 +3069,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2988,13 +3091,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3006,30 +3109,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3045,21 +3149,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3078,14 +3179,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3097,14 +3197,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -3118,9 +3218,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3134,12 +3233,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -3151,9 +3244,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3168,14 +3261,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3187,14 +3279,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -3206,14 +3298,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3222,14 +3313,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -3237,7 +3327,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -3250,11 +3340,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3262,14 +3360,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3281,12 +3379,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3302,7 +3407,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3311,9 +3416,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3329,14 +3433,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3345,20 +3448,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3370,18 +3470,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="'Datos de gráf. dinám. (ocultos)'!$B$8" horiz="1" max="100" page="4" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="'Datos de gráf. dinám. (ocultos)'!$B$8" horiz="1" max="100" page="4" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3394,8 +3488,8 @@
       <xdr:rowOff>295276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>5901</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>2019300</xdr:rowOff>
     </xdr:to>
@@ -3434,8 +3528,8 @@
           <xdr:rowOff>85725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>17</xdr:col>
-          <xdr:colOff>609600</xdr:colOff>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>5902</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>266700</xdr:rowOff>
         </xdr:to>
@@ -3478,17 +3572,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tareas" displayName="Tareas" ref="G5:K25" totalsRowShown="0">
-  <autoFilter ref="G5:K25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tareas" displayName="Tareas" ref="G5:K25" totalsRowShown="0">
+  <autoFilter ref="G5:K25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="G6:J25">
     <sortCondition ref="H5:H25"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="4" name="N.º" dataDxfId="22"/>
-    <tableColumn id="1" name="Fecha de inicio" dataCellStyle="Date"/>
-    <tableColumn id="2" name="Fecha de finalización" dataCellStyle="Date"/>
-    <tableColumn id="3" name="Tarea"/>
-    <tableColumn id="5" name="Duración en días">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="N.º" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fecha de inicio" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Fecha de finalización" dataCellStyle="Date"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tarea"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Duración en días">
       <calculatedColumnFormula>IFERROR(IF(LEN(Tareas[[#This Row],[Fecha de inicio]])=0,"",(INT(Tareas[[#This Row],[Fecha de finalización]])-INT(Tareas[[#This Row],[Fecha de inicio]]))-(INT(Tareas[[#This Row],[Fecha de inicio]])-INT(Tareas[[#This Row],[Fecha de inicio]]))+1),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3497,8 +3591,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Hitos" displayName="Hitos" ref="B5:E20">
-  <autoFilter ref="B5:E20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Hitos" displayName="Hitos" ref="B5:E20">
+  <autoFilter ref="B5:E20" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3508,10 +3602,10 @@
     <sortCondition ref="D6:D16"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="5" name="N.º" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="3" name="Posición" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="1" name="fecha" totalsRowDxfId="17" dataCellStyle="Date"/>
-    <tableColumn id="2" name="Hito" totalsRowFunction="count"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="N.º" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Posición" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="fecha" totalsRowDxfId="17" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Hito" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="Date Tracking Gantt Chart" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3523,24 +3617,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="DatosDeTareasDinámicas" displayName="DatosDeTareasDinámicas" ref="B14:E21">
-  <autoFilter ref="B14:E21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="DatosDeTareasDinámicas" displayName="DatosDeTareasDinámicas" ref="B14:E21">
+  <autoFilter ref="B14:E21" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Tareas" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Tareas" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Fecha de inicio" dataCellStyle="Date">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Fecha de inicio" dataCellStyle="Date">
       <calculatedColumnFormula>IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Duración de la tarea en días" dataDxfId="13">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Duración de la tarea en días" dataDxfId="13">
       <calculatedColumnFormula>IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H6&lt;=$B$12,'Datos del gráfico'!$I6&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="posición" totalsRowFunction="sum" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="posición" totalsRowFunction="sum" dataDxfId="12">
       <calculatedColumnFormula>IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,"",ROW($A1)),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3554,13 +3648,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="HoyResaltado" displayName="HoyResaltado" ref="B3:C5" totalsRowShown="0">
-  <autoFilter ref="B3:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="HoyResaltado" displayName="HoyResaltado" ref="B3:C5" totalsRowShown="0">
+  <autoFilter ref="B3:C5" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="coordenada X para resaltar el día actual" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="coordenada X para resaltar el día actual" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(IF(TODAY()&lt;MIN(DatosDeTareasDinámicas[Fecha de inicio]),MIN($B$11,MIN(DatosDeTareasDinámicas[Fecha de inicio])),TODAY()),TODAY())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="coordenada Y" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="coordenada Y" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(IF(Seguimiento_hoy="Sí",IF(TODAY()&lt;MIN(DatosDeTareasDinámicas[Fecha de inicio]),0,9),0),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3574,20 +3668,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="DatosDeHitoDinámicos" displayName="DatosDeHitoDinámicos" ref="G17:I32">
-  <autoFilter ref="G17:I32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="DatosDeHitoDinámicos" displayName="DatosDeHitoDinámicos" ref="G17:I32">
+  <autoFilter ref="G17:I32" xr:uid="{00000000-0009-0000-0100-000008000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Hitos" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Hitos" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>IFERROR(IF(LEN('Datos del gráfico'!D6)=0,"",IF(AND('Datos del gráfico'!D6&lt;=$B$12,'Datos del gráfico'!D6&gt;=$B$11-$D$11),'Datos del gráfico'!E6,"")),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Fecha" totalsRowDxfId="7" dataCellStyle="Date">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Fecha" totalsRowDxfId="7" dataCellStyle="Date">
       <calculatedColumnFormula>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D6),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LÍNEA BASE" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="LÍNEA BASE" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C6),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3596,12 +3690,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="IncrementoDeDesplazamiento" displayName="IncrementoDeDesplazamiento" ref="B7:B8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="B7:B8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="IncrementoDeDesplazamiento" displayName="IncrementoDeDesplazamiento" ref="B7:B8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="B7:B8" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="incremento de desplazamiento" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="incremento de desplazamiento" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Date Tracking Gantt Chart" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3613,10 +3707,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="IntervaloDelGráfico" displayName="IntervaloDelGráfico" ref="B10:B12" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="B10:B12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="IntervaloDelGráfico" displayName="IntervaloDelGráfico" ref="B10:B12" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="B10:B12" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Intervalo del gráfico" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Intervalo del gráfico" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(IF(LEN(#REF!)=0,End_Date+15,MIN(#REF!)+15),TODAY())</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3625,10 +3719,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Vencimiento" displayName="Vencimiento" ref="D10:D11" totalsRowShown="0">
-  <autoFilter ref="D10:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Vencimiento" displayName="Vencimiento" ref="D10:D11" totalsRowShown="0">
+  <autoFilter ref="D10:D11" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="vencimiento"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="vencimiento"/>
   </tableColumns>
   <tableStyleInfo name="Date Tracking Gantt Chart" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3930,7 +4024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4051,7 +4145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="11">
         <v>1</v>
@@ -4440,10 +4534,10 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Sí,No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4459,13 +4553,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="76" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4545,7 +4641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4600,7 +4696,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f ca="1">IFERROR(IF(TODAY()&lt;MIN(DatosDeTareasDinámicas[Fecha de inicio]),MIN($B$11,MIN(DatosDeTareasDinámicas[Fecha de inicio])),TODAY()),TODAY())</f>
-        <v>43738</v>
+        <v>43710</v>
       </c>
       <c r="C4" s="3">
         <f ca="1">IFERROR(IF(Seguimiento_hoy="Sí",IF(TODAY()&lt;MIN(DatosDeTareasDinámicas[Fecha de inicio]),0,9),0),0)</f>
@@ -4610,7 +4706,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <f ca="1">IFERROR(IF(TODAY()&lt;MIN(DatosDeTareasDinámicas[Fecha de inicio]),MIN($B$11,MIN(DatosDeTareasDinámicas[Fecha de inicio])),TODAY()),TODAY())</f>
-        <v>43738</v>
+        <v>43710</v>
       </c>
       <c r="C5" s="3">
         <f ca="1">IFERROR(IF(Seguimiento_hoy="Sí",IF(TODAY()&lt;MIN(DatosDeTareasDinámicas[Fecha de inicio]),0,9),0),0)</f>
@@ -4630,7 +4726,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4650,7 +4746,7 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <f ca="1">IFERROR(IF(IncrementoDeDesplazamiento[incremento de desplazamiento]=0,Fecha_de_inicio,IF(Fecha_de_inicio+IncrementoDeDesplazamiento[incremento de desplazamiento]*15&lt;Fecha_de_finalización,Fecha_de_inicio+IncrementoDeDesplazamiento[incremento de desplazamiento]*15,Fecha_de_finalización-1)),"")</f>
-        <v>43785</v>
+        <v>43710</v>
       </c>
       <c r="D11">
         <v>45</v>
@@ -4659,7 +4755,7 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f ca="1">IFERROR(IF($B$11+15&lt;Fecha_de_finalización,$B$11+15,Fecha_de_finalización),"")</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4685,11 +4781,11 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</f>
-        <v>Especificacion de Lenguajes a Usar</v>
+        <v>Inicio de Diseño Relacional y Diagrama de Procesos</v>
       </c>
       <c r="C15" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</f>
-        <v>43738</v>
+        <v>43710</v>
       </c>
       <c r="D15" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H6&lt;=$B$12,'Datos del gráfico'!$I6&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K6,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</f>
@@ -4703,11 +4799,11 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H7,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I7,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H7,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G7,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</f>
-        <v>Casos de Uso</v>
+        <v>Modelo Relacional y Diagrama De Procesos.</v>
       </c>
       <c r="C16" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G7,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</f>
-        <v>43738</v>
+        <v>43717</v>
       </c>
       <c r="D16" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H7&lt;=$B$12,'Datos del gráfico'!$I7&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H7,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K7,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</f>
@@ -4727,15 +4823,15 @@
       </c>
       <c r="B17" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H8,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I8,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H8,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G8,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</f>
-        <v>inicio de Contruccion de la Plataforma</v>
+        <v>Identificacion de Sedes y Tablas a Fragmentar</v>
       </c>
       <c r="C17" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G8,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</f>
-        <v>43745</v>
+        <v>43724</v>
       </c>
       <c r="D17" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H8&lt;=$B$12,'Datos del gráfico'!$I8&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H8,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K8,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,"",6),"")</f>
@@ -4757,15 +4853,15 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H9,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I9,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H9,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G9,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</f>
-        <v>Inicio Construccion de Base de Datos En el lenguaje planteado</v>
+        <v>Lista de Sedes y Fragmentaciones Correspondientes</v>
       </c>
       <c r="C18" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G9,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</f>
-        <v>43745</v>
+        <v>43724</v>
       </c>
       <c r="D18" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H9&lt;=$B$12,'Datos del gráfico'!$I9&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H9,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K9,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,"",5),"")</f>
@@ -4773,63 +4869,63 @@
       </c>
       <c r="G18" s="7" t="str">
         <f ca="1">IFERROR(IF(LEN('Datos del gráfico'!D6)=0,"",IF(AND('Datos del gráfico'!D6&lt;=$B$12,'Datos del gráfico'!D6&gt;=$B$11-$D$11),'Datos del gráfico'!E6,"")),"")</f>
-        <v>Presentacion Beta Plataforma (50 - 60 % del proyecto)</v>
+        <v/>
       </c>
       <c r="H18" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D6),2)</f>
-        <v>43768</v>
-      </c>
-      <c r="I18" s="8">
+        <v>43725</v>
+      </c>
+      <c r="I18" s="8" t="str">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C6),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H10,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I10,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H10,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G10,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</f>
-        <v/>
+        <v>Diagrama de Despliegue y Componentes</v>
       </c>
       <c r="C19" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G10,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</f>
-        <v>43785</v>
+        <v>43731</v>
       </c>
       <c r="D19" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H10&lt;=$B$12,'Datos del gráfico'!$I10&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H10,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K10,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="3" t="str">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,"",4),"")</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G19" s="7" t="str">
         <f ca="1">IFERROR(IF(LEN('Datos del gráfico'!D7)=0,"",IF(AND('Datos del gráfico'!D7&lt;=$B$12,'Datos del gráfico'!D7&gt;=$B$11-$D$11),'Datos del gráfico'!E7,"")),"")</f>
-        <v>Fase 2 Programa Completo (80 - 90 % completado)</v>
+        <v/>
       </c>
       <c r="H19" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D7),2)</f>
-        <v>43789</v>
-      </c>
-      <c r="I19" s="8">
+        <v>43725</v>
+      </c>
+      <c r="I19" s="8" t="str">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C7),"")</f>
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H11,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I11,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H11,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G11,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</f>
-        <v/>
+        <v>Especificacion de Lenguajes a Usar</v>
       </c>
       <c r="C20" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G11,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</f>
-        <v>43785</v>
+        <v>43738</v>
       </c>
       <c r="D20" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H11&lt;=$B$12,'Datos del gráfico'!$I11&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H11,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K11,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="3" t="str">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,"",3),"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G20" s="7" t="str">
         <f>IFERROR(IF(LEN('Datos del gráfico'!D8)=0,"",IF(AND('Datos del gráfico'!D8&lt;=$B$12,'Datos del gráfico'!D8&gt;=$B$11-$D$11),'Datos del gráfico'!E8,"")),"")</f>
@@ -4837,29 +4933,29 @@
       </c>
       <c r="H20" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D8),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I20" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C8),"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Datos del gráfico'!$H12,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))=0,"",IF(OR(OFFSET('Datos del gráfico'!$I12,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&lt;=$B$12,OFFSET('Datos del gráfico'!$H12,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tareas[],OFFSET('Datos del gráfico'!$G12,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),4),"")),"")</f>
-        <v/>
+        <v>Casos de Uso</v>
       </c>
       <c r="C21" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,$B$11,INDEX(Tareas[],OFFSET('Datos del gráfico'!$G12,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1),2)),"")</f>
-        <v>43785</v>
+        <v>43738</v>
       </c>
       <c r="D21" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,0,IF(AND('Datos del gráfico'!$H12&lt;=$B$12,'Datos del gráfico'!$I12&gt;=$B$12),ABS(OFFSET('Datos del gráfico'!$H12,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1)-$B$12)+1,OFFSET('Datos del gráfico'!$K12,IncrementoDeDesplazamiento[incremento de desplazamiento],0,1,1))),"")</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="3" t="str">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3">
         <f ca="1">IFERROR(IF(LEN(DatosDeTareasDinámicas[[#This Row],[Tareas]])=0,"",2),"")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G21" s="7" t="str">
         <f>IFERROR(IF(LEN('Datos del gráfico'!D9)=0,"",IF(AND('Datos del gráfico'!D9&lt;=$B$12,'Datos del gráfico'!D9&gt;=$B$11-$D$11),'Datos del gráfico'!E9,"")),"")</f>
@@ -4867,7 +4963,7 @@
       </c>
       <c r="H21" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D9),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I21" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C9),"")</f>
@@ -4881,21 +4977,21 @@
       </c>
       <c r="H22" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D10),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I22" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C10),"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G23" s="7" t="str">
         <f>IFERROR(IF(LEN('Datos del gráfico'!D11)=0,"",IF(AND('Datos del gráfico'!D11&lt;=$B$12,'Datos del gráfico'!D11&gt;=$B$11-$D$11),'Datos del gráfico'!E11,"")),"")</f>
         <v/>
       </c>
       <c r="H23" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D11),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I23" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C11),"")</f>
@@ -4909,21 +5005,21 @@
       </c>
       <c r="H24" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D12),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I24" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C12),"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G25" s="7" t="str">
         <f>IFERROR(IF(LEN('Datos del gráfico'!D13)=0,"",IF(AND('Datos del gráfico'!D13&lt;=$B$12,'Datos del gráfico'!D13&gt;=$B$11-$D$11),'Datos del gráfico'!E13,"")),"")</f>
         <v/>
       </c>
       <c r="H25" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D13),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I25" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C13),"")</f>
@@ -4937,7 +5033,7 @@
       </c>
       <c r="H26" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D14),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I26" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C14),"")</f>
@@ -4951,7 +5047,7 @@
       </c>
       <c r="H27" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D15),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I27" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C15),"")</f>
@@ -4965,7 +5061,7 @@
       </c>
       <c r="H28" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D16),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I28" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C16),"")</f>
@@ -4979,7 +5075,7 @@
       </c>
       <c r="H29" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D17),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I29" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C17),"")</f>
@@ -4993,7 +5089,7 @@
       </c>
       <c r="H30" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D18),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I30" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C18),"")</f>
@@ -5007,7 +5103,7 @@
       </c>
       <c r="H31" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D19),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I31" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C19),"")</f>
@@ -5024,7 +5120,7 @@
       </c>
       <c r="H32" s="23">
         <f ca="1">IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,$B$12,'Datos del gráfico'!$D20),2)</f>
-        <v>43789</v>
+        <v>43725</v>
       </c>
       <c r="I32" s="8" t="str">
         <f>IFERROR(IF(LEN(DatosDeHitoDinámicos[[#This Row],[Hitos]])=0,"",'Datos del gráfico'!$C20),"")</f>
@@ -5056,7 +5152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>